<commit_message>
Add Last Location to Device Report
</commit_message>
<xml_diff>
--- a/templates/export/devices.xlsx
+++ b/templates/export/devices.xlsx
@@ -45,7 +45,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:area(lastCell="R7")</t>
+          <t>jx:area(lastCell="S7")</t>
         </r>
       </text>
     </comment>
@@ -59,7 +59,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>jx:each(items="devices", var="device", lastCell="R7")</t>
+          <t>jx:each(items="devices", var="device", lastCell="S7")</t>
         </r>
       </text>
     </comment>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>Report type:</t>
   </si>
@@ -182,6 +182,12 @@
   </si>
   <si>
     <t>${dateTool.format("dd-MM-YYYY HH:mm a", device.lastUpdate, locale, timezone)}</t>
+  </si>
+  <si>
+    <t>${device.lastLocation}</t>
+  </si>
+  <si>
+    <t>Last Location</t>
   </si>
 </sst>
 </file>
@@ -312,7 +318,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -354,6 +360,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -799,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R999"/>
+  <dimension ref="A1:S999"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R8" sqref="R8"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -822,9 +831,10 @@
     <col min="16" max="16" width="9.83203125" customWidth="1"/>
     <col min="17" max="17" width="7.6640625" customWidth="1"/>
     <col min="18" max="18" width="23.83203125" customWidth="1"/>
+    <col min="19" max="19" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
       <c r="C1" s="3"/>
@@ -834,7 +844,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -848,7 +858,7 @@
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:18" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>34</v>
       </c>
@@ -862,7 +872,7 @@
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="5"/>
       <c r="C4" s="3"/>
@@ -872,7 +882,7 @@
       <c r="G4" s="6"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
       <c r="B5" s="7"/>
       <c r="C5" s="8"/>
@@ -882,11 +892,11 @@
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
     </row>
-    <row r="6" spans="1:18" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+    <row r="6" spans="1:19" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="17"/>
+      <c r="B6" s="18"/>
       <c r="C6" s="9" t="s">
         <v>3</v>
       </c>
@@ -935,12 +945,15 @@
       <c r="R6" s="9" t="s">
         <v>18</v>
       </c>
+      <c r="S6" s="17" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="7" spans="1:18" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+    <row r="7" spans="1:19" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="18"/>
+      <c r="B7" s="19"/>
       <c r="C7" s="12" t="s">
         <v>20</v>
       </c>
@@ -988,6 +1001,9 @@
       </c>
       <c r="R7" s="12" t="s">
         <v>37</v>
+      </c>
+      <c r="S7" s="12" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update device report and add custom alarm report
</commit_message>
<xml_diff>
--- a/templates/export/devices.xlsx
+++ b/templates/export/devices.xlsx
@@ -1,20 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28810"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11213"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/syousuf/code/p/traccar/traccar/templates/export/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85B4E21D-FD7B-6343-8DC2-343FDF248805}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="7720" windowWidth="32200" windowHeight="13280" tabRatio="989"/>
+    <workbookView xWindow="0" yWindow="7720" windowWidth="32200" windowHeight="13280" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,12 +26,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -49,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A7" authorId="0">
+    <comment ref="A7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -121,12 +117,6 @@
     <t>GPS Device Model</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Last Update</t>
-  </si>
-  <si>
     <t>${device.contact}</t>
   </si>
   <si>
@@ -169,9 +159,6 @@
     <t>${device.model}</t>
   </si>
   <si>
-    <t>${device.status}</t>
-  </si>
-  <si>
     <t>Report Date</t>
   </si>
   <si>
@@ -181,19 +168,28 @@
     <t>${dateTool.format("dd-MM-YYYY", device.membershipDate, locale, timezone)}</t>
   </si>
   <si>
-    <t>${dateTool.format("dd-MM-YYYY HH:mm a", device.lastUpdate, locale, timezone)}</t>
-  </si>
-  <si>
     <t>${device.lastLocation}</t>
   </si>
   <si>
     <t>Last Location</t>
+  </si>
+  <si>
+    <t>New Plate Number</t>
+  </si>
+  <si>
+    <t>${device.newPlateNumber}</t>
+  </si>
+  <si>
+    <t>Online Status</t>
+  </si>
+  <si>
+    <t>${device.getOnlineStatus()}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]&quot; h &quot;m&quot; min&quot;"/>
   </numFmts>
@@ -318,7 +314,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -328,9 +324,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="8"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -368,6 +361,12 @@
     </xf>
     <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -471,7 +470,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1028" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -514,7 +519,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1"/>
+        <xdr:cNvPr id="1026" name="shapetype_202" hidden="1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr txBox="1">
           <a:spLocks noSelect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -807,18 +818,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S999"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="S7" sqref="S7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="15" customWidth="1"/>
-    <col min="6" max="6" width="16.83203125" customWidth="1"/>
+    <col min="1" max="1" width="20" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="5" max="5" width="16.83203125" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="21.6640625" customWidth="1"/>
     <col min="9" max="9" width="12.83203125" customWidth="1"/>
@@ -829,181 +841,178 @@
     <col min="14" max="14" width="17.6640625" customWidth="1"/>
     <col min="15" max="15" width="20.6640625" customWidth="1"/>
     <col min="16" max="16" width="9.83203125" customWidth="1"/>
-    <col min="17" max="17" width="7.6640625" customWidth="1"/>
-    <col min="18" max="18" width="23.83203125" customWidth="1"/>
-    <col min="19" max="19" width="36.1640625" customWidth="1"/>
+    <col min="17" max="17" width="23.83203125" customWidth="1"/>
+    <col min="18" max="18" width="36.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
-    <row r="3" spans="1:19" ht="30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
+        <v>32</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
-      <c r="G4" s="6"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="3"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
       <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
     </row>
-    <row r="6" spans="1:19" s="10" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+    <row r="6" spans="1:18" s="9" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="9" t="s">
+      <c r="B6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="C6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="E6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="F6" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="G6" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="9" t="s">
+      <c r="I6" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="L6" s="9" t="s">
+      <c r="L6" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="Q6" s="9" t="s">
+      <c r="Q6" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="R6" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" s="14" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="R6" s="9" t="s">
+      <c r="B7" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="S6" s="17" t="s">
+      <c r="C7" s="12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F7" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="N7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="O7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="P7" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="11" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" s="15" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="O7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="P7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q7" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="R7" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="S7" s="12" t="s">
-        <v>38</v>
+      <c r="R7" s="11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1987,10 +1996,6 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-  </mergeCells>
   <pageMargins left="0.70833333333333304" right="0.70833333333333304" top="0.74791666666666701" bottom="0.74791666666666701" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>